<commit_message>
Added Edit feature scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/DataLMS.xlsx
+++ b/src/test/resources/TestData/DataLMS.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Login" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Class" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>scenarioName</t>
   </si>
@@ -29,13 +30,73 @@
   </si>
   <si>
     <t>Feb@2025</t>
+  </si>
+  <si>
+    <t>ClassDescription</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Recording</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Edit class with valid data</t>
+  </si>
+  <si>
+    <t>appium</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>application testing</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets</t>
+  </si>
+  <si>
+    <t>Class Updated</t>
+  </si>
+  <si>
+    <t>Edit class with invalid data</t>
+  </si>
+  <si>
+    <t>Edit class with mandatory fields</t>
+  </si>
+  <si>
+    <t>Edit class with optional fields</t>
+  </si>
+  <si>
+    <t>selenium</t>
+  </si>
+  <si>
+    <t>web testing</t>
+  </si>
+  <si>
+    <t>Edit class with invalid values in text fields</t>
+  </si>
+  <si>
+    <t>hu(()&amp;&amp;</t>
+  </si>
+  <si>
+    <t>web***(()</t>
+  </si>
+  <si>
+    <t>LOjuuu9900</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -45,6 +106,15 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="2">
@@ -61,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -71,6 +141,15 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -80,6 +159,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -312,4 +395,132 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="31.25"/>
+    <col customWidth="1" min="2" max="2" width="13.5"/>
+    <col customWidth="1" min="4" max="4" width="14.38"/>
+    <col customWidth="1" min="5" max="5" width="29.13"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="E2"/>
+    <hyperlink r:id="rId2" ref="E3"/>
+    <hyperlink r:id="rId3" ref="E5"/>
+  </hyperlinks>
+  <drawing r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Search and pagination class
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/DataLMS.xlsx
+++ b/src/test/resources/TestData/DataLMS.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>scenarioName</t>
   </si>
@@ -47,6 +47,15 @@
     <t>message</t>
   </si>
   <si>
+    <t>BatchName</t>
+  </si>
+  <si>
+    <t>ClassTopic</t>
+  </si>
+  <si>
+    <t>StaffName</t>
+  </si>
+  <si>
     <t>Edit class with valid data</t>
   </si>
   <si>
@@ -90,6 +99,24 @@
   </si>
   <si>
     <t>LOjuuu9900</t>
+  </si>
+  <si>
+    <t>Search with valid batch name</t>
+  </si>
+  <si>
+    <t>Micro service-01</t>
+  </si>
+  <si>
+    <t>Vidhya Test</t>
+  </si>
+  <si>
+    <t>Getha Takur</t>
+  </si>
+  <si>
+    <t>Search with valid class topic</t>
+  </si>
+  <si>
+    <t>Search with valid staff name</t>
   </si>
 </sst>
 </file>
@@ -432,87 +459,138 @@
       <c r="F1" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>